<commit_message>
crop and resize image into square, delete price in the result layout
</commit_message>
<xml_diff>
--- a/Recipes_addimage_url.xlsx
+++ b/Recipes_addimage_url.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J147"/>
+  <dimension ref="A1:K147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,6 +477,11 @@
       <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Image URL</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Resized Image URL</t>
         </is>
       </c>
     </row>
@@ -544,6 +549,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/1.png</t>
         </is>
       </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/1_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -597,6 +607,11 @@
       <c r="J3" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/2.png</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/2_resized.png</t>
         </is>
       </c>
     </row>
@@ -705,6 +720,7 @@
         </is>
       </c>
       <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -757,6 +773,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/4.png</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/4_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -802,6 +823,11 @@
       <c r="J6" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/5.png</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/5_resized.png</t>
         </is>
       </c>
     </row>
@@ -857,6 +883,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/6.png</t>
         </is>
       </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/6_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -901,6 +932,11 @@
       <c r="J8" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/7.png</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/7_resized.png</t>
         </is>
       </c>
     </row>
@@ -956,6 +992,11 @@
       <c r="J9" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/8.png</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/8_resized.png</t>
         </is>
       </c>
     </row>
@@ -1014,6 +1055,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/9.png</t>
         </is>
       </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/9_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1068,6 +1114,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/10.png</t>
         </is>
       </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/10_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1112,6 +1163,11 @@
       <c r="J12" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/11.png</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/11_resized.png</t>
         </is>
       </c>
     </row>
@@ -1163,6 +1219,11 @@
       <c r="J13" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/12.png</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/12_resized.png</t>
         </is>
       </c>
     </row>
@@ -1216,6 +1277,7 @@
         </is>
       </c>
       <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1262,6 +1324,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/14.png</t>
         </is>
       </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/14_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1305,6 +1372,11 @@
       <c r="J16" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/15.png</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/15_resized.png</t>
         </is>
       </c>
     </row>
@@ -1360,6 +1432,11 @@
       <c r="J17" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/16.png</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/16_resized.png</t>
         </is>
       </c>
     </row>
@@ -1436,6 +1513,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/17.png</t>
         </is>
       </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/17_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1502,6 +1584,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/18.png</t>
         </is>
       </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/18_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1554,6 +1641,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/19.png</t>
         </is>
       </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/19_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1592,6 +1684,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/20.png</t>
         </is>
       </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/20_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1629,6 +1726,11 @@
       <c r="J22" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/21.png</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/21_resized.png</t>
         </is>
       </c>
     </row>
@@ -1650,6 +1752,7 @@
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1700,6 +1803,11 @@
       <c r="J24" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/23.png</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/23_resized.png</t>
         </is>
       </c>
     </row>
@@ -1758,6 +1866,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/24.png</t>
         </is>
       </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/24_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1808,6 +1921,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/25.png</t>
         </is>
       </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/25_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1860,6 +1978,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/26.png</t>
         </is>
       </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/26_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1908,6 +2031,11 @@
       <c r="J28" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/27.png</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/27_resized.png</t>
         </is>
       </c>
     </row>
@@ -1966,6 +2094,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/28.png</t>
         </is>
       </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/28_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2020,6 +2153,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/29.png</t>
         </is>
       </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/29_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -2073,6 +2211,11 @@
       <c r="J31" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/30.png</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/30_resized.png</t>
         </is>
       </c>
     </row>
@@ -2134,6 +2277,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/31.png</t>
         </is>
       </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/31_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -2153,6 +2301,7 @@
       <c r="H33" t="inlineStr"/>
       <c r="I33" t="inlineStr"/>
       <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -2211,6 +2360,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/33.png</t>
         </is>
       </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/33_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -2263,6 +2417,11 @@
       <c r="J35" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/34.png</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/34_resized.png</t>
         </is>
       </c>
     </row>
@@ -2328,6 +2487,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/35.png</t>
         </is>
       </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/35_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -2383,6 +2547,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/36.png</t>
         </is>
       </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/36_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -2427,6 +2596,11 @@
       <c r="J38" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/37.png</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/37_resized.png</t>
         </is>
       </c>
     </row>
@@ -2491,6 +2665,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/38.png</t>
         </is>
       </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/38_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -2546,6 +2725,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/39.png</t>
         </is>
       </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/39_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -2588,6 +2772,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/40.png</t>
         </is>
       </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/40_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -2638,6 +2827,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/41.png</t>
         </is>
       </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/41_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2683,6 +2877,11 @@
       <c r="J43" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/42.png</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/42_resized.png</t>
         </is>
       </c>
     </row>
@@ -2742,6 +2941,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/43.png</t>
         </is>
       </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/43_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -2793,6 +2997,11 @@
       <c r="J45" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/44.png</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/44_resized.png</t>
         </is>
       </c>
     </row>
@@ -2848,6 +3057,11 @@
       <c r="J46" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/45.png</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/45_resized.png</t>
         </is>
       </c>
     </row>
@@ -2907,6 +3121,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/46.png</t>
         </is>
       </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/46_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -2957,6 +3176,11 @@
       <c r="J48" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/47.png</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/47_resized.png</t>
         </is>
       </c>
     </row>
@@ -3015,6 +3239,11 @@
       <c r="J49" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/48.png</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/48_resized.png</t>
         </is>
       </c>
     </row>
@@ -3074,6 +3303,11 @@
       <c r="J50" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/49.png</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/49_resized.png</t>
         </is>
       </c>
     </row>
@@ -3135,6 +3369,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/50.png</t>
         </is>
       </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/50_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -3188,6 +3427,11 @@
       <c r="J52" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/51.png</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/51_resized.png</t>
         </is>
       </c>
     </row>
@@ -3246,6 +3490,7 @@
         </is>
       </c>
       <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -3287,6 +3532,11 @@
       <c r="J54" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/53.png</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/53_resized.png</t>
         </is>
       </c>
     </row>
@@ -3344,6 +3594,11 @@
       <c r="J55" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/54.png</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/54_resized.png</t>
         </is>
       </c>
     </row>
@@ -3404,6 +3659,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/55.png</t>
         </is>
       </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/55_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -3461,6 +3721,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/56.png</t>
         </is>
       </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/56_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
@@ -3515,6 +3780,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/57.png</t>
         </is>
       </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/57_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
@@ -3567,6 +3837,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/58.png</t>
         </is>
       </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/58_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
@@ -3622,6 +3897,11 @@
       <c r="J60" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/59.png</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/59_resized.png</t>
         </is>
       </c>
     </row>
@@ -3678,6 +3958,11 @@
       <c r="J61" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/60.png</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/60_resized.png</t>
         </is>
       </c>
     </row>
@@ -3738,6 +4023,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/61.png</t>
         </is>
       </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/61_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="n">
@@ -3794,6 +4084,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/62.png</t>
         </is>
       </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/62_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="n">
@@ -3852,6 +4147,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/63.png</t>
         </is>
       </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/63_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="n">
@@ -3907,6 +4207,11 @@
       <c r="J65" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/64.png</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/64_resized.png</t>
         </is>
       </c>
     </row>
@@ -3967,6 +4272,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/65.png</t>
         </is>
       </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/65_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="n">
@@ -4025,6 +4335,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/66.png</t>
         </is>
       </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/66_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="n">
@@ -4077,6 +4392,11 @@
       <c r="J68" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/67.png</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/67_resized.png</t>
         </is>
       </c>
     </row>
@@ -4134,6 +4454,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/68.png</t>
         </is>
       </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/68_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="n">
@@ -4185,6 +4510,11 @@
       <c r="J70" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/69.png</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/69_resized.png</t>
         </is>
       </c>
     </row>
@@ -4240,6 +4570,7 @@
         </is>
       </c>
       <c r="J71" t="inlineStr"/>
+      <c r="K71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" s="1" t="n">
@@ -4297,6 +4628,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/71.png</t>
         </is>
       </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/71_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="n">
@@ -4354,6 +4690,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/72.png</t>
         </is>
       </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/72_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="n">
@@ -4408,6 +4749,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/73.png</t>
         </is>
       </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/73_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="n">
@@ -4464,6 +4810,11 @@
       <c r="J75" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/74.png</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/74_resized.png</t>
         </is>
       </c>
     </row>
@@ -4528,6 +4879,7 @@
         </is>
       </c>
       <c r="J76" t="inlineStr"/>
+      <c r="K76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" s="1" t="n">
@@ -4589,6 +4941,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/76.png</t>
         </is>
       </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/76_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="1" t="n">
@@ -4644,6 +5001,11 @@
       <c r="J78" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/77.png</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/77_resized.png</t>
         </is>
       </c>
     </row>
@@ -4702,6 +5064,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/78.png</t>
         </is>
       </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/78_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="1" t="n">
@@ -4757,6 +5124,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/79.png</t>
         </is>
       </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/79_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="1" t="n">
@@ -4812,6 +5184,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/80.png</t>
         </is>
       </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/80_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="1" t="n">
@@ -4866,6 +5243,11 @@
       <c r="J82" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/81.png</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/81_resized.png</t>
         </is>
       </c>
     </row>
@@ -4928,6 +5310,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/82.png</t>
         </is>
       </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/82_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="1" t="n">
@@ -4979,6 +5366,11 @@
       <c r="J84" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/83.png</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/83_resized.png</t>
         </is>
       </c>
     </row>
@@ -5038,6 +5430,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/84.png</t>
         </is>
       </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/84_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="1" t="n">
@@ -5095,6 +5492,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/85.png</t>
         </is>
       </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/85_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="1" t="n">
@@ -5145,6 +5547,11 @@
       <c r="J87" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/86.png</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/86_resized.png</t>
         </is>
       </c>
     </row>
@@ -5198,6 +5605,11 @@
       <c r="J88" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/87.png</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/87_resized.png</t>
         </is>
       </c>
     </row>
@@ -5259,6 +5671,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/88.png</t>
         </is>
       </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/88_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
@@ -5313,6 +5730,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/89.png</t>
         </is>
       </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/89_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="n">
@@ -5368,6 +5790,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/90.png</t>
         </is>
       </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/90_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="n">
@@ -5422,6 +5849,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/91.png</t>
         </is>
       </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/91_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -5472,6 +5904,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/92.png</t>
         </is>
       </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/92_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="n">
@@ -5523,6 +5960,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/93.png</t>
         </is>
       </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/93_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="1" t="n">
@@ -5570,6 +6012,11 @@
       <c r="J95" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/94.png</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/94_resized.png</t>
         </is>
       </c>
     </row>
@@ -5633,6 +6080,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/95.png</t>
         </is>
       </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/95_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="1" t="n">
@@ -5690,6 +6142,11 @@
       <c r="J97" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/96.png</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/96_resized.png</t>
         </is>
       </c>
     </row>
@@ -5747,6 +6204,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/97.png</t>
         </is>
       </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/97_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="n">
@@ -5800,6 +6262,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/98.png</t>
         </is>
       </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/98_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="n">
@@ -5849,6 +6316,11 @@
       <c r="J100" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/99.png</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/99_resized.png</t>
         </is>
       </c>
     </row>
@@ -5907,6 +6379,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/100.png</t>
         </is>
       </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/100_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="n">
@@ -5956,6 +6433,11 @@
       <c r="J102" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/101.png</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/101_resized.png</t>
         </is>
       </c>
     </row>
@@ -6011,6 +6493,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/102.png</t>
         </is>
       </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/102_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="n">
@@ -6063,6 +6550,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/103.png</t>
         </is>
       </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/103_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="n">
@@ -6109,6 +6601,11 @@
       <c r="J105" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/104.png</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/104_resized.png</t>
         </is>
       </c>
     </row>
@@ -6165,6 +6662,11 @@
       <c r="J106" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/105.png</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/105_resized.png</t>
         </is>
       </c>
     </row>
@@ -6224,6 +6726,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/106.png</t>
         </is>
       </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/106_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="1" t="n">
@@ -6281,6 +6788,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/107.png</t>
         </is>
       </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/107_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="1" t="n">
@@ -6338,6 +6850,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/108.png</t>
         </is>
       </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/108_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="1" t="n">
@@ -6394,6 +6911,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/109.png</t>
         </is>
       </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/109_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="1" t="n">
@@ -6441,6 +6963,11 @@
       <c r="J111" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/110.png</t>
+        </is>
+      </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/110_resized.png</t>
         </is>
       </c>
     </row>
@@ -6502,6 +7029,11 @@
       <c r="J112" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/111.png</t>
+        </is>
+      </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/111_resized.png</t>
         </is>
       </c>
     </row>
@@ -6567,6 +7099,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/112.png</t>
         </is>
       </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/112_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="1" t="n">
@@ -6622,6 +7159,7 @@
         </is>
       </c>
       <c r="J114" t="inlineStr"/>
+      <c r="K114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" s="1" t="n">
@@ -6675,6 +7213,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/114.png</t>
         </is>
       </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/114_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="1" t="n">
@@ -6715,6 +7258,11 @@
       <c r="J116" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/115.png</t>
+        </is>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/115_resized.png</t>
         </is>
       </c>
     </row>
@@ -6764,6 +7312,11 @@
       <c r="J117" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/116.png</t>
+        </is>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/116_resized.png</t>
         </is>
       </c>
     </row>
@@ -6815,6 +7368,11 @@
       <c r="J118" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/117.png</t>
+        </is>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/117_resized.png</t>
         </is>
       </c>
     </row>
@@ -6874,6 +7432,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/118.png</t>
         </is>
       </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/118_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="1" t="n">
@@ -6929,6 +7492,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/119.png</t>
         </is>
       </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/119_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="1" t="n">
@@ -6983,6 +7551,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/120.png</t>
         </is>
       </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/120_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="1" t="n">
@@ -7035,6 +7608,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/121.png</t>
         </is>
       </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/121_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="1" t="n">
@@ -7082,6 +7660,11 @@
       <c r="J123" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/122.png</t>
+        </is>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/122_resized.png</t>
         </is>
       </c>
     </row>
@@ -7131,6 +7714,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/123.png</t>
         </is>
       </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/123_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="1" t="n">
@@ -7184,6 +7772,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/124.png</t>
         </is>
       </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/124_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="1" t="n">
@@ -7239,6 +7832,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/125.png</t>
         </is>
       </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/125_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="1" t="n">
@@ -7291,6 +7889,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/126.png</t>
         </is>
       </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/126_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="1" t="n">
@@ -7344,6 +7947,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/127.png</t>
         </is>
       </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/127_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="1" t="n">
@@ -7394,6 +8002,11 @@
       <c r="J129" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/128.png</t>
+        </is>
+      </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/128_resized.png</t>
         </is>
       </c>
     </row>
@@ -7447,6 +8060,11 @@
       <c r="J130" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/129.png</t>
+        </is>
+      </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/129_resized.png</t>
         </is>
       </c>
     </row>
@@ -7501,6 +8119,11 @@
       <c r="J131" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/130.png</t>
+        </is>
+      </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/130_resized.png</t>
         </is>
       </c>
     </row>
@@ -7560,6 +8183,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/131.png</t>
         </is>
       </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/131_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="1" t="n">
@@ -7613,6 +8241,11 @@
       <c r="J133" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/132.png</t>
+        </is>
+      </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/132_resized.png</t>
         </is>
       </c>
     </row>
@@ -7671,6 +8304,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/133.png</t>
         </is>
       </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/133_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="1" t="n">
@@ -7721,6 +8359,11 @@
       <c r="J135" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/134.png</t>
+        </is>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/134_resized.png</t>
         </is>
       </c>
     </row>
@@ -7778,6 +8421,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/135.png</t>
         </is>
       </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/135_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="1" t="n">
@@ -7821,6 +8469,11 @@
       <c r="J137" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/136.png</t>
+        </is>
+      </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/136_resized.png</t>
         </is>
       </c>
     </row>
@@ -7868,6 +8521,11 @@
       <c r="J138" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/137.png</t>
+        </is>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/137_resized.png</t>
         </is>
       </c>
     </row>
@@ -7925,6 +8583,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/138.png</t>
         </is>
       </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/138_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="1" t="n">
@@ -7974,6 +8637,11 @@
       <c r="J140" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/139.png</t>
+        </is>
+      </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/139_resized.png</t>
         </is>
       </c>
     </row>
@@ -8031,6 +8699,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/140.png</t>
         </is>
       </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/140_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="1" t="n">
@@ -8082,6 +8755,11 @@
       <c r="J142" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/141.png</t>
+        </is>
+      </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/141_resized.png</t>
         </is>
       </c>
     </row>
@@ -8141,6 +8819,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/142.png</t>
         </is>
       </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/142_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="1" t="n">
@@ -8196,6 +8879,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/143.png</t>
         </is>
       </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/143_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="1" t="n">
@@ -8245,6 +8933,11 @@
       <c r="J145" t="inlineStr">
         <is>
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/144.png</t>
+        </is>
+      </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/144_resized.png</t>
         </is>
       </c>
     </row>
@@ -8299,6 +8992,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/145.png</t>
         </is>
       </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/145_resized.png</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="1" t="n">
@@ -8350,6 +9048,11 @@
           <t>https://cookfull-image.s3.us-west-1.amazonaws.com/146.png</t>
         </is>
       </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>https://cookfull-image.s3.us-west-1.amazonaws.com/146_resized.png</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>